<commit_message>
[22-May-2018] ex4readS : Revisando tema de envío de mail, modif estructura de Puntos
</commit_message>
<xml_diff>
--- a/modelos/Costos/ModelodeCostosSuscripcion.xlsx
+++ b/modelos/Costos/ModelodeCostosSuscripcion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ex4playS\modelos\Costos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CC072C-2182-4D80-8DE7-8C37E0B9271A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31047F57-71DD-4C30-8B08-B7F54B9AD74D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16320" windowHeight="7545" xr2:uid="{4FE205FF-2A75-4CBF-9091-1EF152644ADD}"/>
   </bookViews>
@@ -386,54 +386,54 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="8" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="6" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="42" fontId="7" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="5" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="42" fontId="7" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="7" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="42" fontId="5" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda [0]" xfId="1" builtinId="7"/>
@@ -780,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC0250DD-B991-49A8-9955-70447FAE6308}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,24 +795,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -863,43 +863,43 @@
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="29">
+      <c r="B7" s="20">
         <v>1000</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="21">
         <f>+D3*B7</f>
         <v>50000000</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="21">
         <f>+D7*(1-E45)</f>
         <v>37020777.731092438</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="16" t="s">
+      <c r="B10" s="24"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="12" t="s">
         <v>21</v>
       </c>
     </row>
@@ -907,14 +907,14 @@
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="7">
         <v>3.49E-2</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <f>+B11*D11</f>
         <v>1745</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="29">
         <v>50000</v>
       </c>
     </row>
@@ -922,129 +922,129 @@
       <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="8">
         <v>900</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <f>+B12</f>
         <v>900</v>
       </c>
-      <c r="D12" s="26"/>
+      <c r="D12" s="30"/>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19">
+      <c r="B13" s="13"/>
+      <c r="C13" s="14">
         <f>+C12+C11</f>
         <v>2645</v>
       </c>
-      <c r="D13" s="26"/>
+      <c r="D13" s="30"/>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="9">
         <v>0.19</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="8">
         <f>+C13*B14</f>
         <v>502.55</v>
       </c>
-      <c r="D14" s="26"/>
+      <c r="D14" s="30"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="14">
+      <c r="B15" s="11"/>
+      <c r="C15" s="10">
         <f>+C13+C14</f>
         <v>3147.55</v>
       </c>
-      <c r="D15" s="26"/>
+      <c r="D15" s="30"/>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="26"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="30"/>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="7">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="8">
         <f>+D11*B17</f>
         <v>750</v>
       </c>
-      <c r="D17" s="26"/>
+      <c r="D17" s="30"/>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="7">
         <v>4.1399999999999996E-3</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="8">
         <f>+D11*B18</f>
         <v>206.99999999999997</v>
       </c>
-      <c r="D18" s="26"/>
+      <c r="D18" s="30"/>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="13">
+      <c r="B19" s="9">
         <v>0.15</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="8">
         <f>+C22*B19</f>
         <v>1197.4789915966383</v>
       </c>
-      <c r="D19" s="26"/>
+      <c r="D19" s="30"/>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="14">
+      <c r="B20" s="11"/>
+      <c r="C20" s="10">
         <f>+C19+C18+C17</f>
         <v>2154.4789915966385</v>
       </c>
-      <c r="D20" s="26"/>
+      <c r="D20" s="30"/>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="str">
+      <c r="A21" s="26" t="str">
         <f>+CONCATENATE("Costos Tributarios - Valor de la suscripción sin IVA ",+TEXT(D11/(1+B22),"$ #.#0,00"))</f>
         <v>Costos Tributarios - Valor de la suscripción sin IVA $ 42.016,81</v>
       </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="26"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="30"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B22" s="11">
         <v>0.19</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C22" s="10">
         <f>+D11-(D11/1.19)</f>
         <v>7983.193277310922</v>
       </c>
-      <c r="D22" s="26"/>
+      <c r="D22" s="30"/>
     </row>
     <row r="23" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="28" t="s">
@@ -1052,54 +1052,54 @@
       </c>
       <c r="B23" s="28"/>
       <c r="C23" s="28"/>
-      <c r="D23" s="26"/>
+      <c r="D23" s="30"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="26"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="30"/>
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="26"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="30"/>
     </row>
     <row r="26" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="26"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="30"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="22"/>
-      <c r="C27" s="23">
+      <c r="B27" s="16"/>
+      <c r="C27" s="17">
         <f>+C15+C20+C22+C26</f>
         <v>13285.222268907561</v>
       </c>
-      <c r="D27" s="24">
+      <c r="D27" s="18">
         <f>+D11-C27</f>
         <v>36714.777731092443</v>
       </c>
-      <c r="E27" s="27">
+      <c r="E27" s="19">
         <f>1-(D27/D11)</f>
         <v>0.26570444537815119</v>
       </c>
-      <c r="F27" s="24" t="s">
+      <c r="F27" s="18" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="16" t="s">
+      <c r="B28" s="24"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="12" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1107,14 +1107,14 @@
       <c r="A29" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B29" s="7">
         <v>3.49E-2</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="8">
         <f>+B29*D29</f>
         <v>2443</v>
       </c>
-      <c r="D29" s="25">
+      <c r="D29" s="29">
         <v>70000</v>
       </c>
     </row>
@@ -1122,129 +1122,129 @@
       <c r="A30" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="9">
+      <c r="B30" s="8">
         <v>900</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="8">
         <f>+B30</f>
         <v>900</v>
       </c>
-      <c r="D30" s="26"/>
+      <c r="D30" s="30"/>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="18" t="s">
+      <c r="A31" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="19">
+      <c r="B31" s="13"/>
+      <c r="C31" s="14">
         <f>+C30+C29</f>
         <v>3343</v>
       </c>
-      <c r="D31" s="26"/>
+      <c r="D31" s="30"/>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="13">
+      <c r="B32" s="9">
         <v>0.19</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="8">
         <f>+C31*B32</f>
         <v>635.16999999999996</v>
       </c>
-      <c r="D32" s="26"/>
+      <c r="D32" s="30"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="15"/>
-      <c r="C33" s="14">
+      <c r="B33" s="11"/>
+      <c r="C33" s="10">
         <f>+C31+C32</f>
         <v>3978.17</v>
       </c>
-      <c r="D33" s="26"/>
+      <c r="D33" s="30"/>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="20" t="s">
+      <c r="A34" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="26"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="30"/>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="8">
+      <c r="B35" s="7">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C35" s="8">
         <f>+D29*B35</f>
         <v>1050</v>
       </c>
-      <c r="D35" s="26"/>
+      <c r="D35" s="30"/>
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="8">
+      <c r="B36" s="7">
         <v>4.1399999999999996E-3</v>
       </c>
-      <c r="C36" s="9">
+      <c r="C36" s="8">
         <f>+D29*B36</f>
         <v>289.79999999999995</v>
       </c>
-      <c r="D36" s="26"/>
+      <c r="D36" s="30"/>
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B37" s="13">
+      <c r="B37" s="9">
         <v>0.15</v>
       </c>
-      <c r="C37" s="9">
+      <c r="C37" s="8">
         <f>+C40*B37</f>
         <v>1676.4705882352939</v>
       </c>
-      <c r="D37" s="26"/>
+      <c r="D37" s="30"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
+      <c r="A38" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="15"/>
-      <c r="C38" s="14">
+      <c r="B38" s="11"/>
+      <c r="C38" s="10">
         <f>+C37+C36+C35</f>
         <v>3016.2705882352939</v>
       </c>
-      <c r="D38" s="26"/>
+      <c r="D38" s="30"/>
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="20" t="str">
+      <c r="A39" s="26" t="str">
         <f>+CONCATENATE("Costos Tributarios - Valor de la suscripción sin IVA ",+TEXT(D29/(1+B40),"$ #.#0,00"))</f>
         <v>Costos Tributarios - Valor de la suscripción sin IVA $ 58.823,53</v>
       </c>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="26"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="30"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="15" t="s">
+      <c r="A40" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B40" s="15">
+      <c r="B40" s="11">
         <v>0.19</v>
       </c>
-      <c r="C40" s="14">
+      <c r="C40" s="10">
         <f>+D29-(D29/1.19)</f>
         <v>11176.470588235294</v>
       </c>
-      <c r="D40" s="26"/>
+      <c r="D40" s="30"/>
     </row>
     <row r="41" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="28" t="s">
@@ -1252,49 +1252,53 @@
       </c>
       <c r="B41" s="28"/>
       <c r="C41" s="28"/>
-      <c r="D41" s="26"/>
+      <c r="D41" s="30"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="26"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="30"/>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="26"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="30"/>
     </row>
     <row r="44" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="26"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="30"/>
     </row>
     <row r="45" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="A45" s="21" t="s">
+      <c r="A45" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B45" s="22"/>
-      <c r="C45" s="23">
+      <c r="B45" s="16"/>
+      <c r="C45" s="17">
         <f>+C33+C38+C40+C44</f>
         <v>18170.911176470589</v>
       </c>
-      <c r="D45" s="24">
+      <c r="D45" s="18">
         <f>+D29-C45</f>
         <v>51829.088823529411</v>
       </c>
-      <c r="E45" s="27">
+      <c r="E45" s="19">
         <f>1-(D45/D29)</f>
         <v>0.25958444537815129</v>
       </c>
-      <c r="F45" s="24" t="s">
+      <c r="F45" s="18" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A9:D9"/>
     <mergeCell ref="A41:C41"/>
     <mergeCell ref="D29:D44"/>
     <mergeCell ref="A23:C23"/>
@@ -1303,10 +1307,6 @@
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="A34:C34"/>
     <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A9:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>